<commit_message>
Se le agregaron las acciones para crear la tabla de simbolos de las variables y expresiones las cuales son +,-,/* para realizar los cuadruplos
Se agregaron las acciones en la tabla relacional y se agrego un
ciclo en la parte del sintactico el cual checa las acciones

Se agregan más archivos de programas y uno de xlsx para ver las
tablas que tenemos
</commit_message>
<xml_diff>
--- a/Terminales.xlsx
+++ b/Terminales.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="956" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -163,6 +163,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -246,13 +247,13 @@
   </sheetPr>
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>